<commit_message>
Trying to figure out how to get text = subtitle to display italicized text
</commit_message>
<xml_diff>
--- a/shells.xlsx
+++ b/shells.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbest/Github/ecoquants/findinghal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PikesStuff/github/findinghal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E9D1195-C881-0E44-B172-7FFE45D5E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A65090A-42A5-144D-96D7-4DBF726DE119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-100" windowWidth="38400" windowHeight="21100"/>
+    <workbookView xWindow="-38400" yWindow="-2780" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shells" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -160,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -292,6 +304,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -638,8 +658,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -994,11 +1015,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1063,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="str">
@@ -1071,7 +1092,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="str">
@@ -1099,7 +1120,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="str">
@@ -1128,7 +1149,7 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="str">
@@ -1156,7 +1177,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="str">
@@ -1185,7 +1206,7 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="str">
@@ -1214,7 +1235,7 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="str">
@@ -1243,7 +1264,7 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="str">
@@ -1271,7 +1292,7 @@
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="str">
@@ -1300,7 +1321,7 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="str">
@@ -1328,7 +1349,7 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="str">
@@ -1357,7 +1378,7 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="str">
@@ -1385,7 +1406,7 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C14" t="str">
@@ -1414,7 +1435,7 @@
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C15" t="str">

</xml_diff>